<commit_message>
update UploadPersonnel.java thêm cột thời vụ vào file mẫu
update UploadPersonnel.java thêm cột thời vụ vào file mẫu
</commit_message>
<xml_diff>
--- a/src/main/webapp/TemplateUpload/Template_DSNhanVien.xlsx
+++ b/src/main/webapp/TemplateUpload/Template_DSNhanVien.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>TT</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Số sổ Bảo Hiểm</t>
+  </si>
+  <si>
+    <t>Thời vụ</t>
   </si>
 </sst>
 </file>
@@ -146,7 +149,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ _₫_-;\-* #,##0.00\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="[$-1010000]d/m/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -765,10 +768,10 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1264,30 +1267,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AZ1"/>
+  <dimension ref="A1:BA1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" customWidth="1"/>
-    <col min="11" max="11" width="23" customWidth="1"/>
-    <col min="20" max="20" width="23" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" customWidth="1"/>
-    <col min="27" max="27" width="18.7109375" customWidth="1"/>
-    <col min="28" max="28" width="23.5703125" customWidth="1"/>
-    <col min="29" max="29" width="18.42578125" customWidth="1"/>
-    <col min="30" max="30" width="21.28515625" customWidth="1"/>
-    <col min="31" max="31" width="28" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" customWidth="1"/>
+    <col min="12" max="12" width="23" customWidth="1"/>
+    <col min="21" max="21" width="23" customWidth="1"/>
+    <col min="22" max="22" width="19.140625" customWidth="1"/>
+    <col min="28" max="28" width="18.7109375" customWidth="1"/>
+    <col min="29" max="29" width="23.5703125" customWidth="1"/>
+    <col min="30" max="30" width="18.42578125" customWidth="1"/>
+    <col min="31" max="31" width="21.28515625" customWidth="1"/>
+    <col min="32" max="32" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1297,118 +1301,120 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
       <c r="AR1" s="1"/>
@@ -1420,6 +1426,7 @@
       <c r="AX1" s="1"/>
       <c r="AY1" s="1"/>
       <c r="AZ1" s="1"/>
+      <c r="BA1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update Upload file bỏ số thứ tự
update Upload file bỏ số thứ tự
</commit_message>
<xml_diff>
--- a/src/main/webapp/TemplateUpload/Template_DSNhanVien.xlsx
+++ b/src/main/webapp/TemplateUpload/Template_DSNhanVien.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
-  <si>
-    <t>TT</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Mã số mới</t>
   </si>
@@ -1267,42 +1264,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA1"/>
+  <dimension ref="A1:AZ1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AE14" sqref="AE14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" customWidth="1"/>
-    <col min="12" max="12" width="23" customWidth="1"/>
-    <col min="21" max="21" width="23" customWidth="1"/>
-    <col min="22" max="22" width="19.140625" customWidth="1"/>
-    <col min="28" max="28" width="18.7109375" customWidth="1"/>
-    <col min="29" max="29" width="23.5703125" customWidth="1"/>
-    <col min="30" max="30" width="18.42578125" customWidth="1"/>
-    <col min="31" max="31" width="21.28515625" customWidth="1"/>
-    <col min="32" max="32" width="28" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="23" customWidth="1"/>
+    <col min="20" max="20" width="23" customWidth="1"/>
+    <col min="21" max="21" width="19.140625" customWidth="1"/>
+    <col min="27" max="27" width="18.7109375" customWidth="1"/>
+    <col min="28" max="28" width="23.5703125" customWidth="1"/>
+    <col min="29" max="29" width="18.42578125" customWidth="1"/>
+    <col min="30" max="30" width="21.28515625" customWidth="1"/>
+    <col min="31" max="31" width="28" customWidth="1"/>
+    <col min="32" max="32" width="21.5703125" customWidth="1"/>
+    <col min="33" max="33" width="24.28515625" customWidth="1"/>
+    <col min="34" max="34" width="14.5703125" customWidth="1"/>
+    <col min="35" max="35" width="21.42578125" customWidth="1"/>
+    <col min="36" max="36" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:52" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -1313,10 +1315,10 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -1328,7 +1330,7 @@
       <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="N1" s="3" t="s">
@@ -1343,7 +1345,7 @@
       <c r="Q1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>16</v>
       </c>
       <c r="S1" s="4" t="s">
@@ -1352,10 +1354,10 @@
       <c r="T1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="4" t="s">
         <v>20</v>
       </c>
       <c r="W1" s="4" t="s">
@@ -1367,7 +1369,7 @@
       <c r="Y1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="3" t="s">
         <v>24</v>
       </c>
       <c r="AA1" s="3" t="s">
@@ -1391,19 +1393,19 @@
       <c r="AG1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AH1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AI1" s="3" t="s">
         <v>33</v>
       </c>
       <c r="AJ1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AK1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AL1" s="3" t="s">
         <v>36</v>
       </c>
       <c r="AM1" s="3" t="s">
@@ -1412,9 +1414,7 @@
       <c r="AN1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
       <c r="AR1" s="1"/>
@@ -1426,7 +1426,6 @@
       <c r="AX1" s="1"/>
       <c r="AY1" s="1"/>
       <c r="AZ1" s="1"/>
-      <c r="BA1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update Upload file Hồ sơ nhân sự : thêm 2 trường
update Upload file Hồ sơ nhân sự : thêm 2 trường
</commit_message>
<xml_diff>
--- a/src/main/webapp/TemplateUpload/Template_DSNhanVien.xlsx
+++ b/src/main/webapp/TemplateUpload/Template_DSNhanVien.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Mã số mới</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Ngày đóng bảo hiểm</t>
   </si>
   <si>
-    <t>Thời gian công tác</t>
-  </si>
-  <si>
     <t>Thôn</t>
   </si>
   <si>
@@ -136,19 +133,31 @@
   </si>
   <si>
     <t>Thời vụ</t>
+  </si>
+  <si>
+    <t>Số tài khoản</t>
+  </si>
+  <si>
+    <t>Số sổ hộ khẩu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="10">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ _₫_-;\-* #,##0.00\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="[$-1010000]d/m/yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="dd\/mm\/yyyy"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="0.0000"/>
+    <numFmt numFmtId="172" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,6 +314,38 @@
       <name val=".VnTime"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="56"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="25">
     <fill>
@@ -430,7 +471,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -560,8 +601,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="193">
+  <cellStyleXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -755,8 +807,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -771,8 +827,103 @@
     <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="171" fontId="24" fillId="0" borderId="1" xfId="196" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="1" xfId="196" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="196" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="24" fillId="0" borderId="1" xfId="73" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="196" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="24" fillId="0" borderId="1" xfId="135" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="196" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="196" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="1" xfId="196" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="24" fillId="0" borderId="1" xfId="196" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="196" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="24" fillId="0" borderId="1" xfId="196" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="1" xfId="196" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="196" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="1" xfId="73" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="196" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="24" fillId="0" borderId="1" xfId="196" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="24" fillId="0" borderId="1" xfId="196" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="1" xfId="196" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="26" fillId="0" borderId="1" xfId="188" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="24" fillId="0" borderId="1" xfId="196" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="1" xfId="196" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="24" fillId="0" borderId="1" xfId="196" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="196" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="196" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="24" fillId="0" borderId="1" xfId="196" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="26" fillId="0" borderId="1" xfId="196" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="1" xfId="196" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="172" fontId="24" fillId="0" borderId="1" xfId="196" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="193">
+  <cellStyles count="197">
     <cellStyle name="20% - Accent1 2" xfId="46"/>
     <cellStyle name="20% - Accent1 2 2" xfId="89"/>
     <cellStyle name="20% - Accent1 3" xfId="138"/>
@@ -884,6 +1035,7 @@
     <cellStyle name="Comma 2" xfId="73"/>
     <cellStyle name="Comma 2 2" xfId="116"/>
     <cellStyle name="Comma 2 3" xfId="187"/>
+    <cellStyle name="Comma 2 3 2" xfId="194"/>
     <cellStyle name="Comma 3" xfId="165"/>
     <cellStyle name="Comma 4" xfId="29"/>
     <cellStyle name="Currency 2" xfId="166"/>
@@ -926,10 +1078,13 @@
     <cellStyle name="Neutral 4" xfId="39"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="1"/>
+    <cellStyle name="Normal 10 2" xfId="195"/>
     <cellStyle name="Normal 11" xfId="189"/>
     <cellStyle name="Normal 11 2" xfId="191"/>
     <cellStyle name="Normal 12" xfId="190"/>
     <cellStyle name="Normal 12 2" xfId="192"/>
+    <cellStyle name="Normal 12 3" xfId="196"/>
+    <cellStyle name="Normal 13" xfId="193"/>
     <cellStyle name="Normal 2" xfId="131"/>
     <cellStyle name="Normal 2 2" xfId="88"/>
     <cellStyle name="Normal 2 2 2" xfId="135"/>
@@ -1264,23 +1419,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AZ1"/>
+  <dimension ref="A1:AZ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AE14" sqref="AE14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
     <col min="10" max="10" width="11.85546875" customWidth="1"/>
     <col min="11" max="11" width="23" customWidth="1"/>
+    <col min="18" max="18" width="11.140625" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" customWidth="1"/>
     <col min="20" max="20" width="23" customWidth="1"/>
     <col min="21" max="21" width="19.140625" customWidth="1"/>
+    <col min="26" max="26" width="17.85546875" customWidth="1"/>
     <col min="27" max="27" width="18.7109375" customWidth="1"/>
     <col min="28" max="28" width="23.5703125" customWidth="1"/>
     <col min="29" max="29" width="18.42578125" customWidth="1"/>
@@ -1291,6 +1450,7 @@
     <col min="34" max="34" width="14.5703125" customWidth="1"/>
     <col min="35" max="35" width="21.42578125" customWidth="1"/>
     <col min="36" max="36" width="16.85546875" customWidth="1"/>
+    <col min="38" max="38" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1301,7 +1461,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -1370,51 +1530,53 @@
         <v>23</v>
       </c>
       <c r="Z1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AL1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AO1" s="1"/>
+      <c r="AO1" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
       <c r="AR1" s="1"/>
@@ -1426,6 +1588,60 @@
       <c r="AX1" s="1"/>
       <c r="AY1" s="1"/>
       <c r="AZ1" s="1"/>
+    </row>
+    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A2" s="30"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="23"/>
+      <c r="AB2" s="23"/>
+      <c r="AC2" s="23"/>
+      <c r="AD2" s="23"/>
+      <c r="AE2" s="14"/>
+      <c r="AF2" s="20"/>
+      <c r="AG2" s="26"/>
+      <c r="AH2" s="24"/>
+      <c r="AI2" s="32"/>
+      <c r="AJ2" s="36"/>
+      <c r="AK2" s="31"/>
+      <c r="AL2" s="29"/>
+      <c r="AM2" s="18"/>
+      <c r="AN2" s="28"/>
+      <c r="AO2" s="7"/>
+      <c r="AP2" s="7"/>
+      <c r="AQ2" s="7"/>
+      <c r="AR2" s="7"/>
+      <c r="AS2" s="7"/>
+      <c r="AT2" s="7"/>
+      <c r="AU2" s="7"/>
+      <c r="AV2" s="7"/>
+      <c r="AW2" s="7"/>
+      <c r="AX2" s="7"/>
+      <c r="AY2" s="7"/>
+      <c r="AZ2" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>